<commit_message>
Updated UI with embedded form
</commit_message>
<xml_diff>
--- a/shift.xlsx
+++ b/shift.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="52">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -559,10 +559,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -571,13 +571,13 @@
         <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
         <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
         <v>46</v>
@@ -586,19 +586,19 @@
         <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -609,37 +609,37 @@
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
         <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
         <v>46</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L3" t="s">
         <v>46</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N3" t="s">
         <v>46</v>
@@ -653,10 +653,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -674,7 +674,7 @@
         <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
         <v>46</v>
@@ -683,16 +683,16 @@
         <v>46</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N4" t="s">
         <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -709,7 +709,7 @@
         <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
         <v>46</v>
@@ -721,7 +721,7 @@
         <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
         <v>46</v>
@@ -733,13 +733,13 @@
         <v>46</v>
       </c>
       <c r="M5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="O5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -759,19 +759,19 @@
         <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
         <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
         <v>49</v>
@@ -786,7 +786,7 @@
         <v>46</v>
       </c>
       <c r="O6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -794,13 +794,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -809,31 +809,31 @@
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
         <v>47</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L7" t="s">
         <v>47</v>
       </c>
       <c r="M7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N7" t="s">
         <v>49</v>
       </c>
       <c r="O7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -841,46 +841,46 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
         <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J8" t="s">
         <v>51</v>
       </c>
       <c r="K8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L8" t="s">
         <v>51</v>
       </c>
       <c r="M8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N8" t="s">
         <v>51</v>
       </c>
       <c r="O8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -891,7 +891,7 @@
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -912,10 +912,10 @@
         <v>46</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L9" t="s">
         <v>46</v>
@@ -924,7 +924,7 @@
         <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O9" t="s">
         <v>46</v>
@@ -944,7 +944,7 @@
         <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
         <v>46</v>
@@ -959,22 +959,22 @@
         <v>46</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M10" t="s">
         <v>46</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -982,7 +982,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
@@ -1003,7 +1003,7 @@
         <v>46</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s">
         <v>46</v>
@@ -1018,7 +1018,7 @@
         <v>46</v>
       </c>
       <c r="N11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O11" t="s">
         <v>46</v>
@@ -1029,22 +1029,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
         <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
         <v>46</v>
@@ -1059,10 +1059,10 @@
         <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N12" t="s">
         <v>46</v>
@@ -1076,37 +1076,37 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
         <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I13" t="s">
         <v>46</v>
       </c>
       <c r="J13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M13" t="s">
         <v>46</v>
@@ -1123,10 +1123,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -1135,7 +1135,7 @@
         <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
         <v>46</v>
@@ -1147,16 +1147,16 @@
         <v>46</v>
       </c>
       <c r="J14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N14" t="s">
         <v>46</v>
@@ -1176,10 +1176,10 @@
         <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
         <v>46</v>
@@ -1197,16 +1197,16 @@
         <v>46</v>
       </c>
       <c r="K15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O15" t="s">
         <v>46</v>
@@ -1217,7 +1217,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>46</v>
@@ -1241,22 +1241,22 @@
         <v>46</v>
       </c>
       <c r="J16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M16" t="s">
         <v>46</v>
       </c>
       <c r="N16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1267,22 +1267,22 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
         <v>46</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I17" t="s">
         <v>46</v>
@@ -1297,10 +1297,10 @@
         <v>46</v>
       </c>
       <c r="M17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O17" t="s">
         <v>46</v>
@@ -1311,28 +1311,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
         <v>46</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" t="s">
         <v>46</v>
       </c>
       <c r="I18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J18" t="s">
         <v>46</v>
@@ -1347,7 +1347,7 @@
         <v>46</v>
       </c>
       <c r="N18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O18" t="s">
         <v>46</v>
@@ -1373,22 +1373,22 @@
         <v>46</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s">
         <v>46</v>
       </c>
       <c r="I19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M19" t="s">
         <v>46</v>
@@ -1408,13 +1408,13 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
         <v>46</v>
@@ -1426,7 +1426,7 @@
         <v>46</v>
       </c>
       <c r="I20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" t="s">
         <v>46</v>
@@ -1441,10 +1441,10 @@
         <v>46</v>
       </c>
       <c r="N20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1452,10 +1452,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -1467,31 +1467,31 @@
         <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H21" t="s">
         <v>51</v>
       </c>
       <c r="I21" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J21" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L21" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M21" t="s">
         <v>47</v>
       </c>
       <c r="N21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O21" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1514,7 +1514,7 @@
         <v>46</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H22" t="s">
         <v>47</v>
@@ -1529,7 +1529,7 @@
         <v>46</v>
       </c>
       <c r="L22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M22" t="s">
         <v>46</v>
@@ -1546,7 +1546,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
         <v>46</v>
@@ -1561,19 +1561,19 @@
         <v>47</v>
       </c>
       <c r="G23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s">
         <v>46</v>
       </c>
       <c r="I23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J23" t="s">
         <v>46</v>
       </c>
       <c r="K23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L23" t="s">
         <v>46</v>
@@ -1585,7 +1585,7 @@
         <v>46</v>
       </c>
       <c r="O23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1596,22 +1596,22 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I24" t="s">
         <v>46</v>
@@ -1626,10 +1626,10 @@
         <v>46</v>
       </c>
       <c r="M24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O24" t="s">
         <v>46</v>
@@ -1640,19 +1640,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
         <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G25" t="s">
         <v>46</v>
@@ -1661,25 +1661,25 @@
         <v>46</v>
       </c>
       <c r="I25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" t="s">
         <v>48</v>
       </c>
-      <c r="J25" t="s">
-        <v>46</v>
-      </c>
-      <c r="K25" t="s">
-        <v>46</v>
-      </c>
       <c r="L25" t="s">
         <v>46</v>
       </c>
       <c r="M25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N25" t="s">
         <v>46</v>
       </c>
       <c r="O25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1702,7 +1702,7 @@
         <v>46</v>
       </c>
       <c r="G26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H26" t="s">
         <v>48</v>
@@ -1711,19 +1711,19 @@
         <v>46</v>
       </c>
       <c r="J26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K26" t="s">
         <v>46</v>
       </c>
       <c r="L26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M26" t="s">
         <v>46</v>
       </c>
       <c r="N26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O26" t="s">
         <v>46</v>
@@ -1737,13 +1737,13 @@
         <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
         <v>46</v>
@@ -1770,10 +1770,10 @@
         <v>46</v>
       </c>
       <c r="N27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1781,29 +1781,29 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" t="s">
         <v>48</v>
       </c>
-      <c r="D28" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" t="s">
-        <v>46</v>
-      </c>
       <c r="J28" t="s">
         <v>46</v>
       </c>
@@ -1814,13 +1814,13 @@
         <v>46</v>
       </c>
       <c r="M28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N28" t="s">
         <v>46</v>
       </c>
       <c r="O28" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -1828,19 +1828,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
         <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G29" t="s">
         <v>46</v>
@@ -1849,19 +1849,19 @@
         <v>46</v>
       </c>
       <c r="I29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M29" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="N29" t="s">
         <v>46</v>
@@ -1881,7 +1881,7 @@
         <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
         <v>46</v>
@@ -1905,7 +1905,7 @@
         <v>46</v>
       </c>
       <c r="L30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M30" t="s">
         <v>50</v>
@@ -1922,7 +1922,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
         <v>46</v>
@@ -1937,7 +1937,7 @@
         <v>46</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H31" t="s">
         <v>46</v>
@@ -1946,7 +1946,7 @@
         <v>46</v>
       </c>
       <c r="J31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K31" t="s">
         <v>46</v>
@@ -1955,13 +1955,13 @@
         <v>46</v>
       </c>
       <c r="M31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N31" t="s">
         <v>46</v>
       </c>
       <c r="O31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1972,13 +1972,13 @@
         <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F32" t="s">
         <v>46</v>
@@ -1987,16 +1987,16 @@
         <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J32" t="s">
         <v>46</v>
       </c>
       <c r="K32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L32" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Added current schedule webpage
</commit_message>
<xml_diff>
--- a/shift.xlsx
+++ b/shift.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="53">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -154,7 +154,7 @@
     <t>SaturdayPM</t>
   </si>
   <si>
-    <t xml:space="preserve">     </t>
+    <t>-</t>
   </si>
   <si>
     <t>Server</t>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Expo</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -565,10 +568,10 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
         <v>46</v>
@@ -577,7 +580,7 @@
         <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
         <v>46</v>
@@ -606,7 +609,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -618,34 +621,34 @@
         <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
         <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
         <v>46</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L3" t="s">
         <v>46</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="O3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -653,16 +656,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
         <v>46</v>
@@ -677,7 +680,7 @@
         <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
         <v>46</v>
@@ -686,13 +689,13 @@
         <v>46</v>
       </c>
       <c r="M4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -709,22 +712,22 @@
         <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
         <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
         <v>46</v>
@@ -750,19 +753,19 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
         <v>46</v>
@@ -786,7 +789,7 @@
         <v>46</v>
       </c>
       <c r="O6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -794,37 +797,37 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
         <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
         <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J7" t="s">
         <v>46</v>
       </c>
       <c r="K7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M7" t="s">
         <v>47</v>
@@ -833,7 +836,7 @@
         <v>47</v>
       </c>
       <c r="O7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -841,10 +844,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
         <v>51</v>
@@ -856,13 +859,13 @@
         <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
         <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J8" t="s">
         <v>46</v>
@@ -871,7 +874,7 @@
         <v>46</v>
       </c>
       <c r="L8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" t="s">
         <v>51</v>
@@ -897,10 +900,10 @@
         <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
         <v>46</v>
@@ -924,10 +927,10 @@
         <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -935,13 +938,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
@@ -950,16 +953,16 @@
         <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s">
         <v>46</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
         <v>46</v>
@@ -968,7 +971,7 @@
         <v>46</v>
       </c>
       <c r="M10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N10" t="s">
         <v>46</v>
@@ -982,28 +985,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
         <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
         <v>46</v>
@@ -1038,10 +1041,10 @@
         <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
         <v>47</v>
@@ -1050,7 +1053,7 @@
         <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J12" t="s">
         <v>46</v>
@@ -1059,7 +1062,7 @@
         <v>47</v>
       </c>
       <c r="L12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M12" t="s">
         <v>46</v>
@@ -1088,7 +1091,7 @@
         <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
         <v>46</v>
@@ -1100,13 +1103,13 @@
         <v>46</v>
       </c>
       <c r="J13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M13" t="s">
         <v>46</v>
@@ -1126,7 +1129,7 @@
         <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -1141,13 +1144,13 @@
         <v>46</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" t="s">
         <v>46</v>
@@ -1156,10 +1159,10 @@
         <v>46</v>
       </c>
       <c r="M14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O14" t="s">
         <v>46</v>
@@ -1170,7 +1173,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>46</v>
@@ -1182,13 +1185,13 @@
         <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I15" t="s">
         <v>46</v>
@@ -1197,7 +1200,7 @@
         <v>46</v>
       </c>
       <c r="K15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L15" t="s">
         <v>47</v>
@@ -1206,10 +1209,10 @@
         <v>46</v>
       </c>
       <c r="N15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1226,7 +1229,7 @@
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
         <v>46</v>
@@ -1235,28 +1238,28 @@
         <v>46</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" t="s">
         <v>46</v>
       </c>
       <c r="K16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M16" t="s">
         <v>46</v>
       </c>
       <c r="N16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1267,7 +1270,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
@@ -1282,7 +1285,7 @@
         <v>46</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I17" t="s">
         <v>46</v>
@@ -1297,13 +1300,13 @@
         <v>46</v>
       </c>
       <c r="M17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1311,13 +1314,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>46</v>
@@ -1326,13 +1329,13 @@
         <v>46</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
         <v>46</v>
       </c>
       <c r="I18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J18" t="s">
         <v>46</v>
@@ -1344,7 +1347,7 @@
         <v>46</v>
       </c>
       <c r="M18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N18" t="s">
         <v>46</v>
@@ -1382,7 +1385,7 @@
         <v>46</v>
       </c>
       <c r="J19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K19" t="s">
         <v>46</v>
@@ -1397,7 +1400,7 @@
         <v>46</v>
       </c>
       <c r="O19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1405,7 +1408,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
@@ -1414,28 +1417,28 @@
         <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
         <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
         <v>46</v>
       </c>
       <c r="I20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M20" t="s">
         <v>46</v>
@@ -1452,46 +1455,46 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
         <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K21" t="s">
         <v>51</v>
       </c>
       <c r="L21" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M21" t="s">
         <v>51</v>
       </c>
       <c r="N21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O21" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1499,7 +1502,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
@@ -1508,7 +1511,7 @@
         <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F22" t="s">
         <v>46</v>
@@ -1526,10 +1529,10 @@
         <v>46</v>
       </c>
       <c r="K22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M22" t="s">
         <v>46</v>
@@ -1538,7 +1541,7 @@
         <v>46</v>
       </c>
       <c r="O22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1546,7 +1549,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
@@ -1558,13 +1561,13 @@
         <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G23" t="s">
         <v>46</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I23" t="s">
         <v>46</v>
@@ -1573,7 +1576,7 @@
         <v>46</v>
       </c>
       <c r="K23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L23" t="s">
         <v>46</v>
@@ -1582,7 +1585,7 @@
         <v>47</v>
       </c>
       <c r="N23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O23" t="s">
         <v>46</v>
@@ -1593,10 +1596,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
@@ -1608,7 +1611,7 @@
         <v>46</v>
       </c>
       <c r="G24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H24" t="s">
         <v>46</v>
@@ -1617,10 +1620,10 @@
         <v>46</v>
       </c>
       <c r="J24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L24" t="s">
         <v>46</v>
@@ -1629,10 +1632,10 @@
         <v>46</v>
       </c>
       <c r="N24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1640,37 +1643,37 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" t="s">
         <v>46</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G25" t="s">
         <v>46</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K25" t="s">
         <v>46</v>
       </c>
       <c r="L25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M25" t="s">
         <v>47</v>
@@ -1687,13 +1690,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E26" t="s">
         <v>48</v>
@@ -1702,10 +1705,10 @@
         <v>46</v>
       </c>
       <c r="G26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I26" t="s">
         <v>46</v>
@@ -1714,7 +1717,7 @@
         <v>48</v>
       </c>
       <c r="K26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L26" t="s">
         <v>46</v>
@@ -1737,43 +1740,43 @@
         <v>46</v>
       </c>
       <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" t="s">
+        <v>46</v>
+      </c>
+      <c r="K27" t="s">
+        <v>46</v>
+      </c>
+      <c r="L27" t="s">
+        <v>46</v>
+      </c>
+      <c r="M27" t="s">
         <v>48</v>
       </c>
-      <c r="D27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" t="s">
-        <v>46</v>
-      </c>
-      <c r="H27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" t="s">
-        <v>46</v>
-      </c>
-      <c r="J27" t="s">
-        <v>46</v>
-      </c>
-      <c r="K27" t="s">
-        <v>46</v>
-      </c>
-      <c r="L27" t="s">
-        <v>46</v>
-      </c>
-      <c r="M27" t="s">
-        <v>50</v>
-      </c>
       <c r="N27" t="s">
         <v>46</v>
       </c>
       <c r="O27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1781,7 +1784,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
         <v>46</v>
@@ -1790,28 +1793,28 @@
         <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" t="s">
         <v>48</v>
       </c>
-      <c r="G28" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" t="s">
-        <v>46</v>
-      </c>
       <c r="I28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" t="s">
         <v>48</v>
-      </c>
-      <c r="J28" t="s">
-        <v>46</v>
-      </c>
-      <c r="K28" t="s">
-        <v>48</v>
-      </c>
-      <c r="L28" t="s">
-        <v>46</v>
       </c>
       <c r="M28" t="s">
         <v>46</v>
@@ -1831,7 +1834,7 @@
         <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
@@ -1867,7 +1870,7 @@
         <v>46</v>
       </c>
       <c r="O29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1878,40 +1881,40 @@
         <v>46</v>
       </c>
       <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K30" t="s">
+        <v>46</v>
+      </c>
+      <c r="L30" t="s">
+        <v>46</v>
+      </c>
+      <c r="M30" t="s">
         <v>50</v>
       </c>
-      <c r="D30" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F30" t="s">
-        <v>46</v>
-      </c>
-      <c r="G30" t="s">
-        <v>46</v>
-      </c>
-      <c r="H30" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" t="s">
-        <v>46</v>
-      </c>
-      <c r="J30" t="s">
-        <v>46</v>
-      </c>
-      <c r="K30" t="s">
-        <v>46</v>
-      </c>
-      <c r="L30" t="s">
-        <v>48</v>
-      </c>
-      <c r="M30" t="s">
-        <v>48</v>
-      </c>
       <c r="N30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O30" t="s">
         <v>50</v>
@@ -1922,20 +1925,20 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" t="s">
         <v>48</v>
       </c>
-      <c r="C31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" t="s">
-        <v>46</v>
-      </c>
       <c r="G31" t="s">
         <v>46</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>46</v>
       </c>
       <c r="I31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J31" t="s">
         <v>46</v>
@@ -1958,7 +1961,7 @@
         <v>46</v>
       </c>
       <c r="N31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O31" t="s">
         <v>46</v>
@@ -1969,10 +1972,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D32" t="s">
         <v>46</v>
@@ -1984,10 +1987,10 @@
         <v>46</v>
       </c>
       <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" t="s">
         <v>51</v>
-      </c>
-      <c r="H32" t="s">
-        <v>46</v>
       </c>
       <c r="I32" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Added clock in times
</commit_message>
<xml_diff>
--- a/shift.xlsx
+++ b/shift.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="66">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -157,28 +157,58 @@
     <t>-</t>
   </si>
   <si>
-    <t>1: Server</t>
-  </si>
-  <si>
-    <t>2: Server</t>
-  </si>
-  <si>
-    <t>3: Server</t>
-  </si>
-  <si>
-    <t>4: Server</t>
-  </si>
-  <si>
-    <t>5: Server</t>
-  </si>
-  <si>
-    <t>H/G</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>Expo</t>
+    <t>10:00: 1</t>
+  </si>
+  <si>
+    <t>10:00: 2</t>
+  </si>
+  <si>
+    <t>10:00: 3</t>
+  </si>
+  <si>
+    <t>10:00: 4</t>
+  </si>
+  <si>
+    <t>10:00: 5</t>
+  </si>
+  <si>
+    <t>11:00: H/G</t>
+  </si>
+  <si>
+    <t>10:00: Bar</t>
+  </si>
+  <si>
+    <t>10:00: Expo</t>
+  </si>
+  <si>
+    <t>4:00: 1</t>
+  </si>
+  <si>
+    <t>4:00: 2</t>
+  </si>
+  <si>
+    <t>4:00: 3</t>
+  </si>
+  <si>
+    <t>4:00: 4</t>
+  </si>
+  <si>
+    <t>4:00: 5</t>
+  </si>
+  <si>
+    <t>4:00: H/G</t>
+  </si>
+  <si>
+    <t>4:00: Bar</t>
+  </si>
+  <si>
+    <t>4:00: Expo</t>
+  </si>
+  <si>
+    <t>5:00: 1</t>
+  </si>
+  <si>
+    <t>5:00: 2</t>
   </si>
   <si>
     <t>Name</t>
@@ -521,7 +551,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -571,14 +601,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
       <c r="E2" t="s">
         <v>46</v>
       </c>
@@ -586,13 +616,13 @@
         <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
         <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
         <v>46</v>
@@ -601,13 +631,13 @@
         <v>46</v>
       </c>
       <c r="L2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s">
         <v>46</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="O2" t="s">
         <v>46</v>
@@ -627,11 +657,11 @@
         <v>46</v>
       </c>
       <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
       <c r="G3" t="s">
         <v>46</v>
       </c>
@@ -645,16 +675,16 @@
         <v>46</v>
       </c>
       <c r="K3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
         <v>53</v>
-      </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" t="s">
-        <v>46</v>
       </c>
       <c r="O3" t="s">
         <v>46</v>
@@ -668,7 +698,7 @@
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -677,28 +707,28 @@
         <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
         <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
         <v>46</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="N4" t="s">
         <v>46</v>
@@ -715,31 +745,31 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
-      </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s">
         <v>46</v>
@@ -748,10 +778,10 @@
         <v>46</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="O5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -780,7 +810,7 @@
         <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J6" t="s">
         <v>46</v>
@@ -795,7 +825,7 @@
         <v>46</v>
       </c>
       <c r="N6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="O6" t="s">
         <v>46</v>
@@ -806,46 +836,46 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" t="s">
         <v>53</v>
       </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" t="s">
-        <v>46</v>
-      </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N7" t="s">
         <v>46</v>
       </c>
       <c r="O7" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -853,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>46</v>
@@ -862,37 +892,37 @@
         <v>47</v>
       </c>
       <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" t="s">
         <v>47</v>
       </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="s">
         <v>47</v>
       </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" t="s">
         <v>47</v>
       </c>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" t="s">
-        <v>46</v>
-      </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -906,22 +936,22 @@
         <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
         <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
         <v>49</v>
@@ -930,13 +960,13 @@
         <v>46</v>
       </c>
       <c r="L9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="M9" t="s">
         <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O9" t="s">
         <v>46</v>
@@ -950,13 +980,13 @@
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
         <v>46</v>
@@ -974,13 +1004,13 @@
         <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
         <v>46</v>
       </c>
       <c r="M10" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="N10" t="s">
         <v>46</v>
@@ -994,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
@@ -1012,10 +1042,10 @@
         <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="J11" t="s">
         <v>46</v>
@@ -1024,7 +1054,7 @@
         <v>46</v>
       </c>
       <c r="L11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M11" t="s">
         <v>46</v>
@@ -1041,43 +1071,43 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N12" t="s">
         <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M12" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12" t="s">
-        <v>46</v>
       </c>
       <c r="O12" t="s">
         <v>46</v>
@@ -1088,16 +1118,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
         <v>46</v>
@@ -1118,7 +1148,7 @@
         <v>46</v>
       </c>
       <c r="L13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M13" t="s">
         <v>46</v>
@@ -1138,19 +1168,19 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
         <v>47</v>
       </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>49</v>
-      </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H14" t="s">
         <v>46</v>
@@ -1162,7 +1192,7 @@
         <v>46</v>
       </c>
       <c r="K14" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="L14" t="s">
         <v>46</v>
@@ -1174,7 +1204,7 @@
         <v>46</v>
       </c>
       <c r="O14" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1182,7 +1212,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>46</v>
@@ -1194,19 +1224,19 @@
         <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
         <v>46</v>
       </c>
       <c r="I15" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K15" t="s">
         <v>46</v>
@@ -1232,43 +1262,43 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G16" t="s">
         <v>46</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="L16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M16" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="N16" t="s">
         <v>46</v>
       </c>
       <c r="O16" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1276,43 +1306,43 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17" t="s">
         <v>48</v>
       </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" t="s">
-        <v>46</v>
-      </c>
-      <c r="K17" t="s">
-        <v>46</v>
-      </c>
-      <c r="L17" t="s">
-        <v>46</v>
-      </c>
       <c r="M17" t="s">
         <v>46</v>
       </c>
       <c r="N17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O17" t="s">
         <v>46</v>
@@ -1323,7 +1353,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
         <v>46</v>
@@ -1353,7 +1383,7 @@
         <v>46</v>
       </c>
       <c r="L18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="M18" t="s">
         <v>46</v>
@@ -1373,7 +1403,7 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>46</v>
@@ -1397,7 +1427,7 @@
         <v>46</v>
       </c>
       <c r="K19" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="L19" t="s">
         <v>46</v>
@@ -1417,7 +1447,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
@@ -1432,10 +1462,10 @@
         <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I20" t="s">
         <v>46</v>
@@ -1467,7 +1497,7 @@
         <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
@@ -1479,7 +1509,7 @@
         <v>46</v>
       </c>
       <c r="G21" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="H21" t="s">
         <v>46</v>
@@ -1494,16 +1524,16 @@
         <v>46</v>
       </c>
       <c r="L21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M21" t="s">
         <v>46</v>
       </c>
       <c r="N21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O21" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1514,7 +1544,7 @@
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
         <v>46</v>
@@ -1526,31 +1556,31 @@
         <v>46</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" t="s">
+        <v>63</v>
+      </c>
+      <c r="L22" t="s">
         <v>49</v>
       </c>
-      <c r="I22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J22" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22" t="s">
-        <v>46</v>
-      </c>
-      <c r="L22" t="s">
-        <v>46</v>
-      </c>
       <c r="M22" t="s">
         <v>46</v>
       </c>
       <c r="N22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="O22" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1561,43 +1591,43 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" t="s">
         <v>48</v>
       </c>
-      <c r="D23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" t="s">
-        <v>46</v>
-      </c>
       <c r="I23" t="s">
         <v>46</v>
       </c>
       <c r="J23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L23" t="s">
         <v>46</v>
       </c>
       <c r="M23" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="N23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1611,40 +1641,40 @@
         <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" t="s">
+        <v>46</v>
+      </c>
+      <c r="L24" t="s">
+        <v>46</v>
+      </c>
+      <c r="M24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N24" t="s">
         <v>50</v>
       </c>
-      <c r="G24" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" t="s">
-        <v>48</v>
-      </c>
-      <c r="I24" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" t="s">
-        <v>46</v>
-      </c>
-      <c r="K24" t="s">
-        <v>51</v>
-      </c>
-      <c r="L24" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" t="s">
-        <v>48</v>
-      </c>
-      <c r="N24" t="s">
-        <v>46</v>
-      </c>
       <c r="O24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1652,43 +1682,43 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
       </c>
       <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" t="s">
+        <v>46</v>
+      </c>
+      <c r="M25" t="s">
+        <v>59</v>
+      </c>
+      <c r="N25" t="s">
         <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" t="s">
-        <v>46</v>
-      </c>
-      <c r="I25" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" t="s">
-        <v>46</v>
-      </c>
-      <c r="K25" t="s">
-        <v>46</v>
-      </c>
-      <c r="L25" t="s">
-        <v>46</v>
-      </c>
-      <c r="M25" t="s">
-        <v>46</v>
-      </c>
-      <c r="N25" t="s">
-        <v>46</v>
       </c>
       <c r="O25" t="s">
         <v>46</v>
@@ -1699,37 +1729,37 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" t="s">
+        <v>46</v>
+      </c>
+      <c r="L26" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" t="s">
-        <v>52</v>
-      </c>
-      <c r="I26" t="s">
-        <v>46</v>
-      </c>
-      <c r="J26" t="s">
-        <v>46</v>
-      </c>
-      <c r="K26" t="s">
-        <v>46</v>
-      </c>
-      <c r="L26" t="s">
-        <v>46</v>
       </c>
       <c r="M26" t="s">
         <v>46</v>
@@ -1761,16 +1791,16 @@
         <v>46</v>
       </c>
       <c r="G27" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" t="s">
         <v>52</v>
       </c>
-      <c r="H27" t="s">
-        <v>46</v>
-      </c>
       <c r="I27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" t="s">
         <v>52</v>
-      </c>
-      <c r="J27" t="s">
-        <v>46</v>
       </c>
       <c r="K27" t="s">
         <v>46</v>
@@ -1793,10 +1823,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
         <v>46</v>
@@ -1843,13 +1873,13 @@
         <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
         <v>46</v>
@@ -1861,10 +1891,10 @@
         <v>46</v>
       </c>
       <c r="I29" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="J29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K29" t="s">
         <v>46</v>
@@ -1879,7 +1909,7 @@
         <v>46</v>
       </c>
       <c r="O29" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1896,13 +1926,13 @@
         <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H30" t="s">
         <v>46</v>
@@ -1914,19 +1944,19 @@
         <v>46</v>
       </c>
       <c r="K30" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="L30" t="s">
         <v>46</v>
       </c>
       <c r="M30" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="N30" t="s">
         <v>46</v>
       </c>
       <c r="O30" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -1946,7 +1976,7 @@
         <v>46</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G31" t="s">
         <v>46</v>
@@ -1961,10 +1991,10 @@
         <v>46</v>
       </c>
       <c r="K31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M31" t="s">
         <v>46</v>
@@ -1981,46 +2011,46 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
         <v>54</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G32" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H32" t="s">
         <v>54</v>
       </c>
       <c r="I32" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="J32" t="s">
         <v>54</v>
       </c>
       <c r="K32" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L32" t="s">
         <v>54</v>
       </c>
       <c r="M32" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="N32" t="s">
         <v>54</v>
       </c>
       <c r="O32" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Date Request off
old request off code deprecated
</commit_message>
<xml_diff>
--- a/shift.xlsx
+++ b/shift.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="66">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -886,16 +886,16 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
         <v>63</v>
@@ -904,10 +904,10 @@
         <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K8" t="s">
         <v>46</v>
@@ -916,10 +916,10 @@
         <v>54</v>
       </c>
       <c r="M8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O8" t="s">
         <v>62</v>
@@ -930,43 +930,43 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
         <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K9" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="L9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M9" t="s">
         <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="O9" t="s">
         <v>46</v>
@@ -983,7 +983,7 @@
         <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
@@ -995,16 +995,16 @@
         <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="J10" t="s">
         <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="L10" t="s">
         <v>46</v>
@@ -1039,10 +1039,10 @@
         <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I11" t="s">
         <v>59</v>
@@ -1054,16 +1054,16 @@
         <v>46</v>
       </c>
       <c r="L11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M11" t="s">
         <v>46</v>
       </c>
       <c r="N11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="O11" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1071,7 +1071,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
@@ -1080,7 +1080,7 @@
         <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
         <v>46</v>
@@ -1092,16 +1092,16 @@
         <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K12" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M12" t="s">
         <v>46</v>
@@ -1118,7 +1118,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
@@ -1130,7 +1130,7 @@
         <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
         <v>46</v>
@@ -1145,19 +1145,19 @@
         <v>46</v>
       </c>
       <c r="K13" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="L13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M13" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" t="s">
+        <v>46</v>
+      </c>
+      <c r="O13" t="s">
         <v>56</v>
-      </c>
-      <c r="N13" t="s">
-        <v>46</v>
-      </c>
-      <c r="O13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1165,7 +1165,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>46</v>
@@ -1183,28 +1183,28 @@
         <v>46</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="L14" t="s">
         <v>46</v>
       </c>
       <c r="M14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="N14" t="s">
         <v>46</v>
       </c>
       <c r="O14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1224,7 +1224,7 @@
         <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
         <v>46</v>
@@ -1236,19 +1236,19 @@
         <v>46</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="L15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="M15" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="N15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O15" t="s">
         <v>46</v>
@@ -1262,25 +1262,25 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G16" t="s">
         <v>46</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I16" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="J16" t="s">
         <v>46</v>
@@ -1292,13 +1292,13 @@
         <v>46</v>
       </c>
       <c r="M16" t="s">
+        <v>46</v>
+      </c>
+      <c r="N16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O16" t="s">
         <v>58</v>
-      </c>
-      <c r="N16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1312,7 +1312,7 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
@@ -1321,10 +1321,10 @@
         <v>46</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I17" t="s">
         <v>46</v>
@@ -1339,13 +1339,13 @@
         <v>46</v>
       </c>
       <c r="M17" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="N17" t="s">
         <v>46</v>
       </c>
       <c r="O17" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1362,7 +1362,7 @@
         <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
         <v>46</v>
@@ -1400,7 +1400,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
         <v>46</v>
@@ -1409,7 +1409,7 @@
         <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
         <v>46</v>
@@ -1421,10 +1421,10 @@
         <v>46</v>
       </c>
       <c r="I19" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="J19" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K19" t="s">
         <v>46</v>
@@ -1439,7 +1439,7 @@
         <v>46</v>
       </c>
       <c r="O19" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1450,7 +1450,7 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
         <v>48</v>
@@ -1462,7 +1462,7 @@
         <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="H20" t="s">
         <v>46</v>
@@ -1474,10 +1474,10 @@
         <v>48</v>
       </c>
       <c r="K20" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="L20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M20" t="s">
         <v>46</v>
@@ -1494,22 +1494,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="H21" t="s">
         <v>46</v>
@@ -1527,7 +1527,7 @@
         <v>46</v>
       </c>
       <c r="M21" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="N21" t="s">
         <v>46</v>
@@ -1547,40 +1547,40 @@
         <v>46</v>
       </c>
       <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" t="s">
+        <v>46</v>
+      </c>
+      <c r="M22" t="s">
+        <v>46</v>
+      </c>
+      <c r="N22" t="s">
         <v>47</v>
       </c>
-      <c r="E22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22" t="s">
-        <v>46</v>
-      </c>
-      <c r="L22" t="s">
-        <v>46</v>
-      </c>
-      <c r="M22" t="s">
-        <v>46</v>
-      </c>
-      <c r="N22" t="s">
-        <v>49</v>
-      </c>
       <c r="O22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1588,25 +1588,25 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
         <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
         <v>46</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I23" t="s">
         <v>46</v>
@@ -1618,16 +1618,16 @@
         <v>46</v>
       </c>
       <c r="L23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M23" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="N23" t="s">
         <v>46</v>
       </c>
       <c r="O23" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1638,37 +1638,37 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" t="s">
+        <v>46</v>
+      </c>
+      <c r="L24" t="s">
         <v>50</v>
       </c>
-      <c r="G24" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" t="s">
-        <v>46</v>
-      </c>
-      <c r="K24" t="s">
-        <v>46</v>
-      </c>
-      <c r="L24" t="s">
-        <v>46</v>
-      </c>
       <c r="M24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="N24" t="s">
         <v>46</v>
@@ -1682,13 +1682,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E25" t="s">
         <v>46</v>
@@ -1700,7 +1700,7 @@
         <v>57</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I25" t="s">
         <v>46</v>
@@ -1709,13 +1709,13 @@
         <v>46</v>
       </c>
       <c r="K25" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="L25" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M25" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="N25" t="s">
         <v>46</v>
@@ -1750,19 +1750,19 @@
         <v>46</v>
       </c>
       <c r="I26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" t="s">
+        <v>46</v>
+      </c>
+      <c r="L26" t="s">
+        <v>46</v>
+      </c>
+      <c r="M26" t="s">
         <v>60</v>
-      </c>
-      <c r="J26" t="s">
-        <v>46</v>
-      </c>
-      <c r="K26" t="s">
-        <v>46</v>
-      </c>
-      <c r="L26" t="s">
-        <v>46</v>
-      </c>
-      <c r="M26" t="s">
-        <v>46</v>
       </c>
       <c r="N26" t="s">
         <v>46</v>
@@ -1791,16 +1791,16 @@
         <v>46</v>
       </c>
       <c r="G27" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H27" t="s">
         <v>46</v>
       </c>
       <c r="I27" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="J27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K27" t="s">
         <v>46</v>
@@ -1809,10 +1809,10 @@
         <v>46</v>
       </c>
       <c r="M27" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="N27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O27" t="s">
         <v>60</v>
@@ -1853,7 +1853,7 @@
         <v>46</v>
       </c>
       <c r="L28" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M28" t="s">
         <v>46</v>
@@ -1873,7 +1873,7 @@
         <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
@@ -1888,19 +1888,19 @@
         <v>46</v>
       </c>
       <c r="H29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="I29" t="s">
         <v>46</v>
       </c>
       <c r="J29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K29" t="s">
         <v>46</v>
       </c>
       <c r="L29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M29" t="s">
         <v>46</v>
@@ -1917,10 +1917,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
@@ -1953,7 +1953,7 @@
         <v>46</v>
       </c>
       <c r="N30" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="O30" t="s">
         <v>46</v>
@@ -1964,7 +1964,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
         <v>46</v>
@@ -1979,10 +1979,10 @@
         <v>46</v>
       </c>
       <c r="G31" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="H31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I31" t="s">
         <v>46</v>
@@ -2014,7 +2014,7 @@
         <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D32" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Added not enough staff warning
</commit_message>
<xml_diff>
--- a/shift.xlsx
+++ b/shift.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="68">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -157,6 +157,36 @@
     <t>-</t>
   </si>
   <si>
+    <t>Not Full</t>
+  </si>
+  <si>
+    <t>4:00: 1</t>
+  </si>
+  <si>
+    <t>4:00: 2</t>
+  </si>
+  <si>
+    <t>4:00: 3</t>
+  </si>
+  <si>
+    <t>4:00: 4</t>
+  </si>
+  <si>
+    <t>4:00: 5</t>
+  </si>
+  <si>
+    <t>4:00: H/G</t>
+  </si>
+  <si>
+    <t>4:00: Bar</t>
+  </si>
+  <si>
+    <t>4:00 Runner</t>
+  </si>
+  <si>
+    <t>4:00: Expo</t>
+  </si>
+  <si>
     <t>10:00: 1</t>
   </si>
   <si>
@@ -169,46 +199,22 @@
     <t>10:00: 4</t>
   </si>
   <si>
+    <t>11:00: H/G</t>
+  </si>
+  <si>
+    <t>10:00: Bar</t>
+  </si>
+  <si>
+    <t>10:00: Expo</t>
+  </si>
+  <si>
+    <t>5:00: 1</t>
+  </si>
+  <si>
+    <t>5:00: 2</t>
+  </si>
+  <si>
     <t>10:00: 5</t>
-  </si>
-  <si>
-    <t>11:00: H/G</t>
-  </si>
-  <si>
-    <t>10:00: Bar</t>
-  </si>
-  <si>
-    <t>10:00: Expo</t>
-  </si>
-  <si>
-    <t>4:00: 1</t>
-  </si>
-  <si>
-    <t>4:00: 2</t>
-  </si>
-  <si>
-    <t>4:00: 3</t>
-  </si>
-  <si>
-    <t>4:00: 4</t>
-  </si>
-  <si>
-    <t>4:00: 5</t>
-  </si>
-  <si>
-    <t>4:00: H/G</t>
-  </si>
-  <si>
-    <t>4:00: Bar</t>
-  </si>
-  <si>
-    <t>4:00: Expo</t>
-  </si>
-  <si>
-    <t>5:00: 1</t>
-  </si>
-  <si>
-    <t>5:00: 2</t>
   </si>
   <si>
     <t>Name</t>
@@ -551,10 +557,10 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>33</v>
@@ -604,7 +610,7 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -628,19 +634,19 @@
         <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s">
         <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="N2" t="s">
         <v>46</v>
       </c>
       <c r="O2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -654,13 +660,13 @@
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
         <v>46</v>
@@ -669,16 +675,16 @@
         <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="K3" t="s">
         <v>46</v>
       </c>
       <c r="L3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="M3" t="s">
         <v>46</v>
@@ -695,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -716,25 +722,25 @@
         <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J4" t="s">
         <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="L4" t="s">
         <v>46</v>
       </c>
       <c r="M4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="N4" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="O4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -745,22 +751,22 @@
         <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
         <v>46</v>
@@ -845,13 +851,13 @@
         <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
         <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
         <v>46</v>
@@ -883,46 +889,46 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
         <v>63</v>
       </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" t="s">
         <v>63</v>
       </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" t="s">
-        <v>46</v>
-      </c>
       <c r="K8" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="N8" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="O8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -930,16 +936,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
         <v>46</v>
@@ -948,25 +954,25 @@
         <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
         <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L9" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="M9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N9" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="O9" t="s">
         <v>46</v>
@@ -986,16 +992,16 @@
         <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
         <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I10" t="s">
         <v>46</v>
@@ -1004,7 +1010,7 @@
         <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
         <v>46</v>
@@ -1039,13 +1045,13 @@
         <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
         <v>46</v>
       </c>
       <c r="I11" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
         <v>46</v>
@@ -1092,7 +1098,7 @@
         <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
         <v>46</v>
@@ -1101,13 +1107,13 @@
         <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M12" t="s">
         <v>46</v>
       </c>
       <c r="N12" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="O12" t="s">
         <v>46</v>
@@ -1118,10 +1124,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -1145,7 +1151,7 @@
         <v>46</v>
       </c>
       <c r="K13" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="L13" t="s">
         <v>46</v>
@@ -1154,10 +1160,10 @@
         <v>46</v>
       </c>
       <c r="N13" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="O13" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1168,7 +1174,7 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -1177,7 +1183,7 @@
         <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="G14" t="s">
         <v>46</v>
@@ -1186,25 +1192,25 @@
         <v>46</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="J14" t="s">
         <v>46</v>
       </c>
       <c r="K14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" t="s">
         <v>57</v>
       </c>
-      <c r="L14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M14" t="s">
-        <v>55</v>
-      </c>
-      <c r="N14" t="s">
-        <v>46</v>
-      </c>
       <c r="O14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1218,37 +1224,37 @@
         <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G15" t="s">
         <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="I15" t="s">
         <v>46</v>
       </c>
       <c r="J15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K15" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="L15" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="M15" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="N15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O15" t="s">
         <v>46</v>
@@ -1262,7 +1268,7 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
@@ -1271,19 +1277,19 @@
         <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
         <v>46</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I16" t="s">
         <v>46</v>
       </c>
       <c r="J16" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="K16" t="s">
         <v>46</v>
@@ -1292,13 +1298,13 @@
         <v>46</v>
       </c>
       <c r="M16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N16" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="O16" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1312,7 +1318,7 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
@@ -1321,10 +1327,10 @@
         <v>46</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="I17" t="s">
         <v>46</v>
@@ -1336,16 +1342,16 @@
         <v>46</v>
       </c>
       <c r="L17" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="M17" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="N17" t="s">
         <v>46</v>
       </c>
       <c r="O17" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1356,13 +1362,13 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
         <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
         <v>46</v>
@@ -1371,7 +1377,7 @@
         <v>46</v>
       </c>
       <c r="H18" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="I18" t="s">
         <v>46</v>
@@ -1380,7 +1386,7 @@
         <v>46</v>
       </c>
       <c r="K18" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L18" t="s">
         <v>46</v>
@@ -1409,7 +1415,7 @@
         <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
         <v>46</v>
@@ -1421,10 +1427,10 @@
         <v>46</v>
       </c>
       <c r="I19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="J19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K19" t="s">
         <v>46</v>
@@ -1450,10 +1456,10 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
         <v>46</v>
@@ -1462,7 +1468,7 @@
         <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
         <v>46</v>
@@ -1471,13 +1477,13 @@
         <v>46</v>
       </c>
       <c r="J20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K20" t="s">
         <v>46</v>
       </c>
       <c r="L20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M20" t="s">
         <v>46</v>
@@ -1486,7 +1492,7 @@
         <v>46</v>
       </c>
       <c r="O20" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1494,19 +1500,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
         <v>50</v>
       </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G21" t="s">
         <v>46</v>
@@ -1533,7 +1539,7 @@
         <v>46</v>
       </c>
       <c r="O21" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1553,34 +1559,34 @@
         <v>46</v>
       </c>
       <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" t="s">
+        <v>46</v>
+      </c>
+      <c r="M22" t="s">
+        <v>49</v>
+      </c>
+      <c r="N22" t="s">
+        <v>46</v>
+      </c>
+      <c r="O22" t="s">
         <v>50</v>
-      </c>
-      <c r="G22" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" t="s">
-        <v>57</v>
-      </c>
-      <c r="J22" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22" t="s">
-        <v>46</v>
-      </c>
-      <c r="L22" t="s">
-        <v>46</v>
-      </c>
-      <c r="M22" t="s">
-        <v>46</v>
-      </c>
-      <c r="N22" t="s">
-        <v>47</v>
-      </c>
-      <c r="O22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1588,10 +1594,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
         <v>46</v>
@@ -1612,7 +1618,7 @@
         <v>46</v>
       </c>
       <c r="J23" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="K23" t="s">
         <v>46</v>
@@ -1621,7 +1627,7 @@
         <v>46</v>
       </c>
       <c r="M23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="N23" t="s">
         <v>46</v>
@@ -1635,46 +1641,46 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
         <v>46</v>
       </c>
       <c r="I24" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="J24" t="s">
         <v>46</v>
       </c>
       <c r="K24" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M24" t="s">
         <v>50</v>
       </c>
-      <c r="M24" t="s">
-        <v>56</v>
-      </c>
       <c r="N24" t="s">
         <v>46</v>
       </c>
       <c r="O24" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1685,34 +1691,34 @@
         <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F25" t="s">
         <v>46</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I25" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J25" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="K25" t="s">
         <v>46</v>
       </c>
       <c r="L25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M25" t="s">
         <v>46</v>
@@ -1735,13 +1741,13 @@
         <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G26" t="s">
         <v>46</v>
@@ -1762,10 +1768,10 @@
         <v>46</v>
       </c>
       <c r="M26" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="N26" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="O26" t="s">
         <v>46</v>
@@ -1779,7 +1785,7 @@
         <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
         <v>46</v>
@@ -1791,16 +1797,16 @@
         <v>46</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="H27" t="s">
         <v>46</v>
       </c>
       <c r="I27" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="J27" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="K27" t="s">
         <v>46</v>
@@ -1812,10 +1818,10 @@
         <v>46</v>
       </c>
       <c r="N27" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="O27" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1826,7 +1832,7 @@
         <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
         <v>46</v>
@@ -1853,7 +1859,7 @@
         <v>46</v>
       </c>
       <c r="L28" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="M28" t="s">
         <v>46</v>
@@ -1879,7 +1885,7 @@
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F29" t="s">
         <v>46</v>
@@ -1888,7 +1894,7 @@
         <v>46</v>
       </c>
       <c r="H29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I29" t="s">
         <v>46</v>
@@ -1909,7 +1915,7 @@
         <v>46</v>
       </c>
       <c r="O29" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1917,19 +1923,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G30" t="s">
         <v>46</v>
@@ -1944,13 +1950,13 @@
         <v>46</v>
       </c>
       <c r="K30" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="L30" t="s">
         <v>46</v>
       </c>
       <c r="M30" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="N30" t="s">
         <v>46</v>
@@ -1970,7 +1976,7 @@
         <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E31" t="s">
         <v>46</v>
@@ -1979,10 +1985,10 @@
         <v>46</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H31" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="I31" t="s">
         <v>46</v>
@@ -1997,13 +2003,13 @@
         <v>46</v>
       </c>
       <c r="M31" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="N31" t="s">
         <v>46</v>
       </c>
       <c r="O31" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2014,43 +2020,43 @@
         <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E32" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G32" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="H32" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="I32" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="J32" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K32" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="L32" t="s">
         <v>46</v>
       </c>
       <c r="M32" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="N32" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="O32" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>